<commit_message>
Aggiunti grafici e capitolo sulle prestazioni
</commit_message>
<xml_diff>
--- a/Prestazioni.xlsx
+++ b/Prestazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CJM\GitHub\BitonicSortVSQuickSort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DE013B-D5BF-4882-B772-1761F46A0948}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992EE1A3-099E-473B-BF41-8B7B7A85D4ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{EE9A0081-2AE7-4863-ADA8-4EDD32C60109}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3450" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="87">
   <si>
     <t>"-O0"</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Quick Sort (32P)</t>
+  </si>
+  <si>
+    <t>QuickSort</t>
+  </si>
+  <si>
+    <t>BitonicSort</t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2071,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3070,16 +3075,13 @@
                   <a:buFontTx/>
                   <a:buNone/>
                   <a:tabLst/>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="1">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:sysClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="it-IT" sz="1000"/>
@@ -3253,16 +3255,13 @@
                   <a:buFontTx/>
                   <a:buNone/>
                   <a:tabLst/>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr b="1">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:sysClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="it-IT" sz="1000"/>
@@ -4731,6 +4730,916 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1" u="sng"/>
+              <a:t>Speedup -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" u="sng" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" u="sng"/>
+              <a:t>BitonicSort</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1582408446787787E-2"/>
+          <c:y val="0.11039239552856471"/>
+          <c:w val="0.90479986636618126"/>
+          <c:h val="0.80267956895898407"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Grafici!$Z$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BitonicSort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Grafici!$Y$9:$Y$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Grafici!$Z$9:$Z$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.0207750000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7983999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7065999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88870000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5363</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E05C-44F1-BB93-A638EC7967D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="421616048"/>
+        <c:axId val="421613424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="421616048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" b="1"/>
+                  <a:t>N. Processori</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="421613424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="421613424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" b="1"/>
+                  <a:t>Tempo di esecuzione (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="421616048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speedup - QuickSort</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.6493894655942908E-2"/>
+          <c:y val="0.14182547460014441"/>
+          <c:w val="0.88004339174434942"/>
+          <c:h val="0.78355204119031041"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Grafici!$Z$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QuickSort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Grafici!$Y$17:$Y$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Grafici!$Z$17:$Z$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.56859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55366666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34415000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40579999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55430000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-06F7-4EAD-B809-FA8849845CFD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="495309464"/>
+        <c:axId val="495307496"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="495309464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>N. Processori</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495307496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="495307496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT"/>
+                  <a:t>Tempo di esecuzione (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495309464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="1"/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4972,6 +5881,86 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8542,6 +9531,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -8796,6 +10791,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>757488</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>183230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>395538</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>54643</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C4B30E4-F4BC-4BC7-8DF5-E425056E2BF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Grafico 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D658B8-E4AB-4648-98AD-C2531C62919A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -45912,10 +47979,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEB27E3-A315-4FEA-BBF5-F028C77DE9B6}">
-  <dimension ref="A8:Q43"/>
+  <dimension ref="A8:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="Z3" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45923,9 +47990,11 @@
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>131072</v>
       </c>
@@ -45968,8 +48037,11 @@
       <c r="Q8" s="3">
         <v>8388608</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Z8" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -46032,8 +48104,15 @@
         <f>Test!CB11</f>
         <v>0.56859999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Y9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <f>H9</f>
+        <v>7.0207750000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -46096,8 +48175,15 @@
         <f>MAX(Test!CB27,Test!CB28)</f>
         <v>0.55366666666666664</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Y10" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z10">
+        <f>H10</f>
+        <v>3.7983999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>4</v>
       </c>
@@ -46160,8 +48246,15 @@
         <f>Test!CB52</f>
         <v>0.53425</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Y11" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z11">
+        <f>H11</f>
+        <v>1.7065999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -46224,8 +48317,15 @@
         <f>Test!CB95</f>
         <v>0.34415000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Y12" s="3">
+        <v>8</v>
+      </c>
+      <c r="Z12">
+        <f>H12</f>
+        <v>0.88870000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>16</v>
       </c>
@@ -46288,8 +48388,15 @@
         <f>Test!CB175</f>
         <v>0.40579999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Y13" s="3">
+        <v>16</v>
+      </c>
+      <c r="Z13">
+        <f>H13</f>
+        <v>0.5363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>32</v>
       </c>
@@ -46350,6 +48457,72 @@
       </c>
       <c r="Q14">
         <f>Test!CB327</f>
+        <v>0.55430000000000001</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>32</v>
+      </c>
+      <c r="Z14">
+        <f>H14</f>
+        <v>0.5151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z16" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <f>Q9</f>
+        <v>0.56859999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y18" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z18">
+        <f>Q10</f>
+        <v>0.55366666666666664</v>
+      </c>
+    </row>
+    <row r="19" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y19" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z19">
+        <f>Q11</f>
+        <v>0.53425</v>
+      </c>
+    </row>
+    <row r="20" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y20" s="3">
+        <v>8</v>
+      </c>
+      <c r="Z20">
+        <f>Q12</f>
+        <v>0.34415000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y21" s="3">
+        <v>16</v>
+      </c>
+      <c r="Z21">
+        <f>Q13</f>
+        <v>0.40579999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="25:26" x14ac:dyDescent="0.25">
+      <c r="Y22" s="3">
+        <v>32</v>
+      </c>
+      <c r="Z22">
+        <f>Q14</f>
         <v>0.55430000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiunti grafici di speedup
</commit_message>
<xml_diff>
--- a/Prestazioni.xlsx
+++ b/Prestazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CJM\GitHub\BitonicSortVSQuickSort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992EE1A3-099E-473B-BF41-8B7B7A85D4ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3EE915-6114-4C0B-A422-F9063454A591}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{EE9A0081-2AE7-4863-ADA8-4EDD32C60109}"/>
   </bookViews>
@@ -4848,6 +4848,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Grafici!$Y$9:$Y$14</c:f>
@@ -4909,8 +4967,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -5210,7 +5269,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5223,7 +5282,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" u="sng"/>
               <a:t>Speedup - QuickSort</a:t>
             </a:r>
           </a:p>
@@ -5242,7 +5301,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="sng" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -5299,6 +5358,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Grafici!$Y$17:$Y$22</c:f>
@@ -5360,8 +5477,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -47981,8 +48099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEB27E3-A315-4FEA-BBF5-F028C77DE9B6}">
   <dimension ref="A8:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z3" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="AL14" sqref="AL14"/>
+    <sheetView tabSelected="1" topLeftCell="Y24" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="AL35" sqref="AL35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>